<commit_message>
These are current versions as of 28/04/18 @10:25pm
</commit_message>
<xml_diff>
--- a/Docs/featureRank.xlsx
+++ b/Docs/featureRank.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzh94\Desktop\Repo\phishing_Detect\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OSSResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FAC62057-32AF-4442-9BC0-3146E69036C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B148E9-7EAC-46AB-9CEA-BF093E38A501}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="5715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Feature Position</t>
   </si>
@@ -66,34 +66,27 @@
     <t>Set E</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>Count</t>
   </si>
   <si>
-    <t>Average</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>FPR</t>
   </si>
   <si>
-    <t>Running Total</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>TPR</t>
   </si>
   <si>
-    <t>Count</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Features</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>AUC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -102,13 +95,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,13 +132,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,44 +172,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Fig.1</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t>: </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Performance</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> Comparesion</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -248,7 +197,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -360,63 +309,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$F$3:$F$7</c:f>
@@ -569,70 +461,8 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$F$3:$F$7</c:f>
@@ -740,7 +570,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="326541072"/>
@@ -754,7 +584,6 @@
         <c:axId val="326541072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -800,7 +629,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="326538448"/>
@@ -842,7 +671,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -872,7 +701,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -917,14 +746,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Fig. 2: Feature Counts vs Accuracy</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Feature</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1600">
-              <a:effectLst/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Count vs Accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -932,8 +761,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19278536823213308"/>
-          <c:y val="4.9812235009085402E-2"/>
+          <c:x val="0.42063720908125918"/>
+          <c:y val="2.7777777777777776E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -961,7 +790,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -976,11 +805,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$28</c:f>
+              <c:f>Sheet1!$G$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Features</c:v>
+                  <c:v>Count</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1009,89 +838,32 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$E$29:$E$33</c:f>
+              <c:f>Sheet1!$F$10:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Set A</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Set B</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Set C</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>Set D</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Set E</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Set B</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$29:$F$33</c:f>
+              <c:f>Sheet1!$G$10:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1099,16 +871,16 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1116,7 +888,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0883-4641-B983-D2C5D10F7302}"/>
+              <c16:uniqueId val="{00000000-A893-4E51-88AE-BCB271E6180C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1128,8 +900,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="507470520"/>
-        <c:axId val="507468880"/>
+        <c:axId val="422673168"/>
+        <c:axId val="422675136"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1139,7 +911,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$28</c:f>
+              <c:f>Sheet1!$H$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1174,30 +946,30 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$E$29:$E$33</c:f>
+              <c:f>Sheet1!$F$10:$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Set A</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Set B</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Set C</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>Set D</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Set E</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Set B</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set D</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$29:$G$33</c:f>
+              <c:f>Sheet1!$H$10:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1205,16 +977,16 @@
                   <c:v>0.50419999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.76770000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.94120000000000004</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.95730000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.96199999999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.76770000000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.95730000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1222,191 +994,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0883-4641-B983-D2C5D10F7302}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Recall</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$E$29:$E$33</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Set A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Set C</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Set E</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Set B</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$29:$H$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.56179999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.92400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94140000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.77869999999999995</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.93920000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0883-4641-B983-D2C5D10F7302}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$28</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Precision</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$E$29:$E$33</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Set A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Set C</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Set E</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Set B</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$29:$I$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.44650000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.94030000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.97089999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.71509999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96220000000000006</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0883-4641-B983-D2C5D10F7302}"/>
+              <c16:uniqueId val="{00000001-A893-4E51-88AE-BCB271E6180C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1418,11 +1006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="507471504"/>
-        <c:axId val="507472488"/>
+        <c:axId val="417012960"/>
+        <c:axId val="417014600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="507470520"/>
+        <c:axId val="422673168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,10 +1030,9 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="@" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1476,15 +1063,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507468880"/>
+        <c:crossAx val="422675136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="507468880"/>
+        <c:axId val="422675136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,18 +1125,17 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507470520"/>
+        <c:crossAx val="422673168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="507472488"/>
+        <c:axId val="417014600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1587,15 +1173,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507471504"/>
+        <c:crossAx val="417012960"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="507471504"/>
+        <c:axId val="417012960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1190,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="507472488"/>
+        <c:crossAx val="417014600"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1642,19 +1229,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1679,7 +1259,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1687,6 +1267,478 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16067340255034493"/>
+          <c:y val="9.543875981019613E-2"/>
+          <c:w val="0.68316885389326332"/>
+          <c:h val="0.74744944839745242"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.18E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.86E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2407</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54039999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.56179999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77869999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93920000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94140000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CA32-4B74-9AC7-EE9D31DD561F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1154039023"/>
+        <c:axId val="1151362863"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1154039023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>False Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39666922165702745"/>
+              <c:y val="0.89984019238974455"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1151362863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1151362863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.6111173603299587E-2"/>
+              <c:y val="0.26431262480330731"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1154039023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.85346662917135363"/>
+          <c:y val="0.3648931222532058"/>
+          <c:w val="0.10738429377743711"/>
+          <c:h val="5.4612032719211077E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1770,6 +1822,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2789,20 +2881,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2829,27 +3441,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83A5588D-1DD0-4476-8AF6-17B71B105040}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2863,7 +3477,149 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1362074</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0C1FA03-DF3E-490F-B2BC-FAA6256D78BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.14762</cdr:x>
+      <cdr:y>0.93126</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.85804</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB4E288-1C7F-4CB0-BBCC-7A859112322C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="787400" y="3321911"/>
+          <a:ext cx="3789363" cy="245202"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Fig. 2 ROC Curve for Random</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Forest Classifier.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.3375</cdr:x>
+      <cdr:y>0.0203</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6125</cdr:x>
+      <cdr:y>0.07868</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5307688B-FF3B-47A8-859D-81B545A543AE}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1800225" y="76200"/>
+          <a:ext cx="1466850" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>ROC Curve</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3163,21 +3919,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="23.125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3217,8 +3973,17 @@
       <c r="J2" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A14" si="0">SUM(A2+1)</f>
         <v>2</v>
@@ -3247,8 +4012,15 @@
       <c r="J3" s="3">
         <v>0.50419999999999998</v>
       </c>
+      <c r="K3" s="4">
+        <v>2.18E-2</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.56179999999999997</v>
+      </c>
+      <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3277,8 +4049,15 @@
       <c r="J4" s="3">
         <v>0.76770000000000005</v>
       </c>
+      <c r="K4" s="4">
+        <v>2.86E-2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.77869999999999995</v>
+      </c>
+      <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3307,8 +4086,15 @@
       <c r="J5" s="3">
         <v>0.94120000000000004</v>
       </c>
+      <c r="K5" s="4">
+        <v>4.5400000000000003E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3337,8 +4123,15 @@
       <c r="J6" s="3">
         <v>0.95730000000000004</v>
       </c>
+      <c r="K6" s="4">
+        <v>0.2407</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.93920000000000003</v>
+      </c>
+      <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3367,8 +4160,15 @@
       <c r="J7" s="3">
         <v>0.96199999999999997</v>
       </c>
+      <c r="K7" s="4">
+        <v>0.54039999999999999</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3383,7 +4183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3397,8 +4197,15 @@
       <c r="D9">
         <v>13</v>
       </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3412,8 +4219,18 @@
       <c r="D10">
         <v>9</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <f>J3</f>
+        <v>0.50419999999999998</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3427,8 +4244,18 @@
       <c r="D11">
         <v>24</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3">
+        <v>21</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" ref="H11:H14" si="1">J4</f>
+        <v>0.76770000000000005</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3442,8 +4269,18 @@
       <c r="D12">
         <v>16</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="3">
+        <v>8</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.94120000000000004</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3457,8 +4294,18 @@
       <c r="D13">
         <v>27</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="3">
+        <v>30</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95730000000000004</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3472,10 +4319,20 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.96199999999999997</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" ref="A15:A31" si="1">SUM(A14+1)</f>
+        <f t="shared" ref="A15:A31" si="2">SUM(A14+1)</f>
         <v>14</v>
       </c>
       <c r="B15" s="1">
@@ -3488,9 +4345,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
@@ -3503,9 +4360,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
@@ -3518,9 +4375,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
@@ -3530,9 +4387,9 @@
         <v>7.0872399999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B19" s="1">
@@ -3542,9 +4399,9 @@
         <v>5.5085999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B20" s="1">
@@ -3554,9 +4411,9 @@
         <v>5.4679100000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="B21" s="1">
@@ -3566,9 +4423,9 @@
         <v>5.2706999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="B22" s="1">
@@ -3578,9 +4435,9 @@
         <v>4.9244500000000004E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="B23" s="1">
@@ -3590,9 +4447,9 @@
         <v>4.8989000000000003E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="B24" s="1">
@@ -3602,9 +4459,9 @@
         <v>4.725E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="B25" s="1">
@@ -3614,9 +4471,9 @@
         <v>4.69682E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="B26" s="1">
@@ -3626,9 +4483,9 @@
         <v>4.4351299999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="B27" s="1">
@@ -3638,9 +4495,9 @@
         <v>3.3386800000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="B28" s="1">
@@ -3649,22 +4506,10 @@
       <c r="C28" s="1">
         <v>3.2946999999999998E-3</v>
       </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-      <c r="H28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -3673,25 +4518,10 @@
       <c r="C29" s="1">
         <v>2.8825000000000001E-3</v>
       </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29">
-        <v>4</v>
-      </c>
-      <c r="G29">
-        <v>0.50419999999999998</v>
-      </c>
-      <c r="H29">
-        <v>0.56179999999999997</v>
-      </c>
-      <c r="I29">
-        <v>0.44650000000000001</v>
-      </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="B30" s="1">
@@ -3700,25 +4530,10 @@
       <c r="C30" s="1">
         <v>2.4533599999999999E-3</v>
       </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30">
-        <v>8</v>
-      </c>
-      <c r="G30">
-        <v>0.94120000000000004</v>
-      </c>
-      <c r="H30">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="I30">
-        <v>0.94030000000000002</v>
-      </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="B31" s="1">
@@ -3727,61 +4542,11 @@
       <c r="C31" s="1">
         <v>1.8933400000000001E-3</v>
       </c>
-      <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31">
-        <v>16</v>
-      </c>
-      <c r="G31">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="H31">
-        <v>0.94140000000000001</v>
-      </c>
-      <c r="I31">
-        <v>0.97089999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32">
-        <v>21</v>
-      </c>
-      <c r="G32">
-        <v>0.76770000000000005</v>
-      </c>
-      <c r="H32">
-        <v>0.77869999999999995</v>
-      </c>
-      <c r="I32">
-        <v>0.71509999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33">
-        <v>30</v>
-      </c>
-      <c r="G33">
-        <v>0.95730000000000004</v>
-      </c>
-      <c r="H33">
-        <v>0.93920000000000003</v>
-      </c>
-      <c r="I33">
-        <v>0.96220000000000006</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="E29:I33">
-    <sortCondition ref="F28"/>
+  <sortState ref="C2:C31">
+    <sortCondition descending="1" ref="C2:C31"/>
   </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Contains both old and new values for FPR, TPR.
</commit_message>
<xml_diff>
--- a/Docs/featureRank.xlsx
+++ b/Docs/featureRank.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OSSResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\phishing_Detect-master\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B148E9-7EAC-46AB-9CEA-BF093E38A501}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D1AF29-1851-4732-96AF-41AB6DA748B1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="5715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Feature Position</t>
   </si>
@@ -76,6 +76,30 @@
   </si>
   <si>
     <t>AUC</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Manual ROC</t>
+  </si>
+  <si>
+    <t>Auto ROC</t>
+  </si>
+  <si>
+    <t>Auto ROC in Reverse</t>
   </si>
 </sst>
 </file>
@@ -1284,19 +1308,64 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Manual ROC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.16067340255034493"/>
-          <c:y val="9.543875981019613E-2"/>
-          <c:w val="0.68316885389326332"/>
-          <c:h val="0.74744944839745242"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1305,7 +1374,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$2</c:f>
+              <c:f>Sheet1!$U$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1315,7 +1384,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1324,8 +1393,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1334,55 +1403,60 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$7</c:f>
+              <c:f>Sheet1!$T$42:$T$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>0.53029999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2424</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3599999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2.18E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.86E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.5400000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.2407</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.54039999999999999</c:v>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$7</c:f>
+              <c:f>Sheet1!$U$42:$U$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.56179999999999997</c:v>
+                  <c:v>0.51190000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77869999999999995</c:v>
+                  <c:v>0.78300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92400000000000004</c:v>
+                  <c:v>0.91539999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.93920000000000003</c:v>
+                  <c:v>0.94140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.94140000000000001</c:v>
+                  <c:v>0.94789999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1390,7 +1464,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CA32-4B74-9AC7-EE9D31DD561F}"/>
+              <c16:uniqueId val="{00000000-05B6-4DF7-87CD-A990140505CD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1402,11 +1476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1154039023"/>
-        <c:axId val="1151362863"/>
+        <c:axId val="991612352"/>
+        <c:axId val="999503632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1154039023"/>
+        <c:axId val="991612352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,69 +1500,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>False Positive Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.39666922165702745"/>
-              <c:y val="0.89984019238974455"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1498,133 +1509,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1151362863"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1151362863"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>True Positive Rate</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="3.6111173603299587E-2"/>
-              <c:y val="0.26431262480330731"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1651,7 +1537,69 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1154039023"/>
+        <c:crossAx val="999503632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="999503632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="991612352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1663,54 +1611,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.85346662917135363"/>
-          <c:y val="0.3648931222532058"/>
-          <c:w val="0.10738429377743711"/>
-          <c:h val="5.4612032719211077E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -1738,7 +1645,947 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Auto ROC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8672897196261688E-2"/>
+          <c:y val="0.14959251491617445"/>
+          <c:w val="0.88073862642169731"/>
+          <c:h val="0.6571889868628813"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$42:$K$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4500000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$42:$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>0.46689999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75749999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93930000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96630000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97809999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B295-4973-B2CF-1E94CBF5C70B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="993094288"/>
+        <c:axId val="999514000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="993094288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fasle Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="999514000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="999514000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="993094288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Original ROC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.18E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.86E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2407</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54039999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.56179999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77869999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93920000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94140000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3CC3-49E4-B01A-D3EFEC8E52F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="925775648"/>
+        <c:axId val="999820976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="925775648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>False Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="999820976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="999820976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3888888888888888E-2"/>
+              <c:y val="0.31539592166178637"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="925775648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1862,6 +2709,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2882,7 +3809,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2893,7 +3820,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2909,25 +3836,25 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2939,7 +3866,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2947,11 +3874,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -2983,45 +3910,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3033,26 +3950,22 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -3082,13 +3995,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3098,7 +4013,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3107,131 +4022,142 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3252,7 +4178,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -3260,7 +4186,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3273,17 +4199,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3291,10 +4206,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -3315,7 +4230,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3324,13 +4239,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3344,26 +4260,27 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3380,9 +4297,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3395,8 +4312,1046 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3405,16 +5360,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3441,16 +5396,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3479,23 +5434,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1362074</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0C1FA03-DF3E-490F-B2BC-FAA6256D78BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69CF9A6D-BD07-45FF-AC31-E89E73D96157}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3513,113 +5468,79 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.14762</cdr:x>
-      <cdr:y>0.93126</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.85804</cdr:x>
-      <cdr:y>1</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DB4E288-1C7F-4CB0-BBCC-7A859112322C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BDD26FB-89B1-4415-8F5A-429408DE3109}"/>
             </a:ext>
           </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="787400" y="3321911"/>
-          <a:ext cx="3789363" cy="245202"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>Fig. 2 ROC Curve for Random</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t> Forest Classifier.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1200">
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.3375</cdr:x>
-      <cdr:y>0.0203</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.6125</cdr:x>
-      <cdr:y>0.07868</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5307688B-FF3B-47A8-859D-81B545A543AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DC4160-55DD-4947-B891-E3877CEF4471}"/>
             </a:ext>
           </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1800225" y="76200"/>
-          <a:ext cx="1466850" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>ROC Curve</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3919,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4543,6 +6464,307 @@
         <v>1.8933400000000001E-3</v>
       </c>
     </row>
+    <row r="40" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P40" t="s">
+        <v>24</v>
+      </c>
+      <c r="S40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U41" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+      <c r="P42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="3"/>
+      <c r="S42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T42" s="3">
+        <v>0.53029999999999999</v>
+      </c>
+      <c r="U42" s="3">
+        <v>0.51190000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0.42830000000000001</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0.51190000000000002</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0.48809999999999998</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0.46689999999999998</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0.49080000000000001</v>
+      </c>
+      <c r="O43" s="3">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="P43" s="3">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T43" s="3">
+        <v>0.2424</v>
+      </c>
+      <c r="U43" s="3">
+        <v>0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0.74739999999999995</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0.75749999999999995</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0.77029999999999998</v>
+      </c>
+      <c r="O44" s="3">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="P44" s="3">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T44" s="3">
+        <v>6.0600000000000001E-2</v>
+      </c>
+      <c r="U44" s="3">
+        <v>0.91539999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.92130000000000001</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="K45" s="3">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0.93930000000000002</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0.92730000000000001</v>
+      </c>
+      <c r="O45" s="3">
+        <v>8.4500000000000006E-2</v>
+      </c>
+      <c r="P45" s="3">
+        <v>0.93930000000000002</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T45" s="3">
+        <v>3.3599999999999998E-2</v>
+      </c>
+      <c r="U45" s="3">
+        <v>0.94140000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0.95589999999999997</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0.9486</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0.95540000000000003</v>
+      </c>
+      <c r="K46" s="3">
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0.96630000000000005</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0.95379999999999998</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0.21690000000000001</v>
+      </c>
+      <c r="P46" s="3">
+        <v>0.75749999999999995</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T46" s="3">
+        <v>2.18E-2</v>
+      </c>
+      <c r="U46" s="3">
+        <v>0.94789999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="F47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0.97109999999999996</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0.94789999999999996</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0.95930000000000004</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0.96489999999999998</v>
+      </c>
+      <c r="K47" s="3">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0.97809999999999997</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="P47" s="3">
+        <v>0.46689999999999998</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3">
+        <v>0</v>
+      </c>
+      <c r="U47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:21" x14ac:dyDescent="0.25">
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="C2:C31">
     <sortCondition descending="1" ref="C2:C31"/>

</xml_diff>

<commit_message>
Merge the 2 excel files
</commit_message>
<xml_diff>
--- a/Docs/featureRank.xlsx
+++ b/Docs/featureRank.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\phishing_Detect-master\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhaohe Zhang\Desktop\git_repo\phishing_Detect\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D1AF29-1851-4732-96AF-41AB6DA748B1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EB8C7667-869B-4A99-8DEC-D7E35BC3D0D9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="5715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12300" windowHeight="5712" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Feature Position</t>
   </si>
@@ -101,12 +105,52 @@
   <si>
     <t>Auto ROC in Reverse</t>
   </si>
+  <si>
+    <t>TP</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>FN</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>TN</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>FP</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confusion Matrix Set A: </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confusion Matrix Set B: </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confusion Matrix Set C: </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confusion Matrix Set D: </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confusion Matrix Set E: </t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,16 +164,29 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -152,11 +209,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -164,8 +274,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2589,6 +2725,360 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>RoC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Binary Classify data'!$M$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'[1]Binary Classify data'!$L$8:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.44642857142857145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18181818181818182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5326633165829151E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4925124792013313E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9669421487603308E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'[1]Binary Classify data'!$M$8:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="1">
+                  <c:v>0.42831215970961889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71485148514851482</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92139737991266379</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95594713656387664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97111111111111115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B44-4D4D-AA00-09CAC204E729}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="499022976"/>
+        <c:axId val="499025928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="499022976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="499025928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="499025928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="499022976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2789,6 +3279,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4841,6 +5371,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5543,6 +6589,110 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDC86774-90A8-46B5-BC33-2F38C4F1D3A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Binary Classify data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="M7" t="str">
+            <v>TPR</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="L9">
+            <v>0.44642857142857145</v>
+          </cell>
+          <cell r="M9">
+            <v>0.42831215970961889</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="L10">
+            <v>0.18181818181818182</v>
+          </cell>
+          <cell r="M10">
+            <v>0.71485148514851482</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="L11">
+            <v>6.5326633165829151E-2</v>
+          </cell>
+          <cell r="M11">
+            <v>0.92139737991266379</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="L12">
+            <v>4.4925124792013313E-2</v>
+          </cell>
+          <cell r="M12">
+            <v>0.95594713656387664</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="L13">
+            <v>3.9669421487603308E-2</v>
+          </cell>
+          <cell r="M13">
+            <v>0.97111111111111115</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5842,19 +6992,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E47" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5868,7 +7018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5904,7 +7054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A14" si="0">SUM(A2+1)</f>
         <v>2</v>
@@ -5941,7 +7091,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -5978,7 +7128,7 @@
       </c>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6015,7 +7165,7 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6052,7 +7202,7 @@
       </c>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6089,7 +7239,7 @@
       </c>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6104,7 +7254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6126,7 +7276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6151,7 +7301,7 @@
         <v>0.50419999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6176,7 +7326,7 @@
         <v>0.76770000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6201,7 +7351,7 @@
         <v>0.94120000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6226,7 +7376,7 @@
         <v>0.95730000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6251,7 +7401,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" ref="A15:A31" si="2">SUM(A14+1)</f>
         <v>14</v>
@@ -6266,7 +7416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -6281,7 +7431,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -6296,7 +7446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -6308,7 +7458,7 @@
         <v>7.0872399999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -6320,7 +7470,7 @@
         <v>5.5085999999999998E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -6332,7 +7482,7 @@
         <v>5.4679100000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -6344,7 +7494,7 @@
         <v>5.2706999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -6356,7 +7506,7 @@
         <v>4.9244500000000004E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -6368,7 +7518,7 @@
         <v>4.8989000000000003E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -6380,7 +7530,7 @@
         <v>4.725E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -6392,7 +7542,7 @@
         <v>4.69682E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -6404,7 +7554,7 @@
         <v>4.4351299999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -6416,7 +7566,7 @@
         <v>3.3386800000000001E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -6428,7 +7578,7 @@
         <v>3.2946999999999998E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -6440,7 +7590,7 @@
         <v>2.8825000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -6452,7 +7602,7 @@
         <v>2.4533599999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -6464,7 +7614,7 @@
         <v>1.8933400000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:21" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
         <v>23</v>
       </c>
@@ -6475,7 +7625,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
         <v>4</v>
@@ -6513,7 +7663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -6539,7 +7689,7 @@
         <v>0.51190000000000002</v>
       </c>
     </row>
-    <row r="43" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F43" s="3" t="s">
         <v>8</v>
       </c>
@@ -6583,7 +7733,7 @@
         <v>0.78300000000000003</v>
       </c>
     </row>
-    <row r="44" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F44" s="3" t="s">
         <v>9</v>
       </c>
@@ -6627,7 +7777,7 @@
         <v>0.91539999999999999</v>
       </c>
     </row>
-    <row r="45" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F45" s="3" t="s">
         <v>10</v>
       </c>
@@ -6671,7 +7821,7 @@
         <v>0.94140000000000001</v>
       </c>
     </row>
-    <row r="46" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F46" s="3" t="s">
         <v>11</v>
       </c>
@@ -6715,7 +7865,7 @@
         <v>0.94789999999999996</v>
       </c>
     </row>
-    <row r="47" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F47" s="3" t="s">
         <v>12</v>
       </c>
@@ -6757,7 +7907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:21" x14ac:dyDescent="0.3">
       <c r="K48" s="3">
         <v>0</v>
       </c>
@@ -6773,4 +7923,572 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777480CF-F7BB-4881-86BB-5A5A820AF980}">
+  <dimension ref="C7:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.42830000000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.51190000000000002</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.48809999999999998</v>
+      </c>
+      <c r="H9" s="5">
+        <v>236</v>
+      </c>
+      <c r="I9" s="5">
+        <v>315</v>
+      </c>
+      <c r="J9" s="5">
+        <v>279</v>
+      </c>
+      <c r="K9" s="5">
+        <v>225</v>
+      </c>
+      <c r="L9" s="5">
+        <f>K9 /( SUM(J9:K9))</f>
+        <v>0.44642857142857145</v>
+      </c>
+      <c r="M9" s="5">
+        <f>H9/(SUM(H9:I9))</f>
+        <v>0.42831215970961889</v>
+      </c>
+      <c r="N9" s="5">
+        <f xml:space="preserve"> (SUM(H9,J9))/1055</f>
+        <v>0.4881516587677725</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.74739999999999995</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.76870000000000005</v>
+      </c>
+      <c r="H10" s="5">
+        <v>361</v>
+      </c>
+      <c r="I10" s="5">
+        <v>144</v>
+      </c>
+      <c r="J10" s="5">
+        <v>450</v>
+      </c>
+      <c r="K10" s="5">
+        <v>100</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L13" si="0">K10 /( SUM(J10:K10))</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="M10" s="5">
+        <f>H10/(SUM(H10:I10))</f>
+        <v>0.71485148514851482</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" ref="N10:N13" si="1" xml:space="preserve"> (SUM(H10,J10))/1055</f>
+        <v>0.76872037914691949</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.92130000000000001</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.91539999999999999</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="H11" s="5">
+        <v>422</v>
+      </c>
+      <c r="I11" s="5">
+        <v>36</v>
+      </c>
+      <c r="J11" s="5">
+        <v>558</v>
+      </c>
+      <c r="K11" s="5">
+        <v>39</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5326633165829151E-2</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" ref="M11:M13" si="2">H11/(SUM(H11:I11))</f>
+        <v>0.92139737991266379</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.92890995260663511</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.95589999999999997</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.9486</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.95540000000000003</v>
+      </c>
+      <c r="H12" s="5">
+        <v>434</v>
+      </c>
+      <c r="I12" s="5">
+        <v>20</v>
+      </c>
+      <c r="J12" s="5">
+        <v>574</v>
+      </c>
+      <c r="K12" s="5">
+        <v>27</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4925124792013313E-2</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" si="2"/>
+        <v>0.95594713656387664</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.95545023696682463</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.97109999999999996</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.94789999999999996</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.95930000000000004</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.96489999999999998</v>
+      </c>
+      <c r="H13" s="5">
+        <v>437</v>
+      </c>
+      <c r="I13" s="5">
+        <v>13</v>
+      </c>
+      <c r="J13" s="5">
+        <v>581</v>
+      </c>
+      <c r="K13" s="5">
+        <v>24</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" si="0"/>
+        <v>3.9669421487603308E-2</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97111111111111115</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.96492890995260661</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="H16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D18" s="12">
+        <v>236</v>
+      </c>
+      <c r="E18" s="12">
+        <v>225</v>
+      </c>
+      <c r="F18" s="12">
+        <v>461</v>
+      </c>
+      <c r="H18" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I18" s="13">
+        <v>361</v>
+      </c>
+      <c r="J18" s="13">
+        <v>100</v>
+      </c>
+      <c r="K18" s="13">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>315</v>
+      </c>
+      <c r="E19" s="12">
+        <v>279</v>
+      </c>
+      <c r="F19" s="12">
+        <v>594</v>
+      </c>
+      <c r="H19" s="13">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13">
+        <v>144</v>
+      </c>
+      <c r="J19" s="13">
+        <v>450</v>
+      </c>
+      <c r="K19" s="13">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="12">
+        <v>551</v>
+      </c>
+      <c r="E20" s="12">
+        <v>504</v>
+      </c>
+      <c r="F20" s="12">
+        <v>1055</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="13">
+        <v>505</v>
+      </c>
+      <c r="J20" s="13">
+        <v>550</v>
+      </c>
+      <c r="K20" s="13">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="H22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J23" s="13">
+        <v>1</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="13">
+        <v>422</v>
+      </c>
+      <c r="E24" s="13">
+        <v>39</v>
+      </c>
+      <c r="F24" s="13">
+        <v>461</v>
+      </c>
+      <c r="H24" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I24" s="13">
+        <v>434</v>
+      </c>
+      <c r="J24" s="13">
+        <v>27</v>
+      </c>
+      <c r="K24" s="13">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="13">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13">
+        <v>36</v>
+      </c>
+      <c r="E25" s="13">
+        <v>558</v>
+      </c>
+      <c r="F25" s="13">
+        <v>594</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
+      <c r="I25" s="13">
+        <v>20</v>
+      </c>
+      <c r="J25" s="13">
+        <v>574</v>
+      </c>
+      <c r="K25" s="13">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="13">
+        <v>458</v>
+      </c>
+      <c r="E26" s="13">
+        <v>597</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1055</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="13">
+        <v>454</v>
+      </c>
+      <c r="J26" s="13">
+        <v>601</v>
+      </c>
+      <c r="K26" s="13">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13">
+        <v>-1</v>
+      </c>
+      <c r="E29" s="13">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D30" s="13">
+        <v>437</v>
+      </c>
+      <c r="E30" s="13">
+        <v>24</v>
+      </c>
+      <c r="F30" s="13">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="13">
+        <v>1</v>
+      </c>
+      <c r="D31" s="13">
+        <v>13</v>
+      </c>
+      <c r="E31" s="13">
+        <v>581</v>
+      </c>
+      <c r="F31" s="13">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="13">
+        <v>450</v>
+      </c>
+      <c r="E32" s="13">
+        <v>605</v>
+      </c>
+      <c r="F32" s="13">
+        <v>1055</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="C28:F28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>